<commit_message>
Binaries for version 0.0.6.
</commit_message>
<xml_diff>
--- a/Bin/Test/UnitTest 2013 00.xlsx
+++ b/Bin/Test/UnitTest 2013 00.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="19980" windowHeight="8070" tabRatio="258"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="19980" windowHeight="8070" tabRatio="258" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test_1.1" sheetId="5" r:id="rId1"/>
     <sheet name="Test_1.2" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="59">
   <si>
     <t>Target</t>
   </si>
@@ -154,12 +153,6 @@
   </si>
   <si>
     <t>Unit2/ENV</t>
-  </si>
-  <si>
-    <t>Unit3/ENV</t>
-  </si>
-  <si>
-    <t>Unit4/ENV</t>
   </si>
   <si>
     <t>Test 1.1</t>
@@ -176,6 +169,30 @@
   <si>
     <t>This is my message 2 :
 "It BREAKS!"</t>
+  </si>
+  <si>
+    <t>Section1/MPU_A</t>
+  </si>
+  <si>
+    <t>Section2/MPU_A</t>
+  </si>
+  <si>
+    <t>Section1/MPU_T</t>
+  </si>
+  <si>
+    <t>Section2/MPU_T</t>
+  </si>
+  <si>
+    <t>Section1/ENV</t>
+  </si>
+  <si>
+    <t>Section2/ENV</t>
+  </si>
+  <si>
+    <t>Section3/ENV</t>
+  </si>
+  <si>
+    <t>Section4/ENV</t>
   </si>
 </sst>
 </file>
@@ -310,9 +327,6 @@
       </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <color theme="0"/>
@@ -338,6 +352,9 @@
           <bgColor theme="7"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -417,7 +434,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_Action_1.1" displayName="Table_Action_1.1" ref="B5:G17" totalsRowCount="1">
   <autoFilter ref="B5:G16"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="7" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="7" totalsRowDxfId="6"/>
     <tableColumn id="2" name="Path"/>
     <tableColumn id="6" name="Location"/>
     <tableColumn id="3" name="STEP 1" totalsRowLabel="200"/>
@@ -431,10 +448,10 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_Check_1.1" displayName="Table_Check_1.1" ref="B19:G25" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="6">
-    <tableColumn id="1" name="Target" dataDxfId="6"/>
+    <tableColumn id="1" name="Target" dataDxfId="5"/>
     <tableColumn id="2" name="Location"/>
     <tableColumn id="6" name="Colonne1"/>
-    <tableColumn id="3" name="STEP 1" headerRowDxfId="5"/>
+    <tableColumn id="3" name="STEP 1" headerRowDxfId="4"/>
     <tableColumn id="4" name="Column1"/>
     <tableColumn id="5" name="Column2"/>
   </tableColumns>
@@ -469,7 +486,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table_Action_1.2" displayName="Table_Action_1.2" ref="B5:G17" totalsRowCount="1">
   <autoFilter ref="B5:G16"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="3" totalsRowDxfId="0"/>
     <tableColumn id="2" name="Path"/>
     <tableColumn id="6" name="Location"/>
     <tableColumn id="3" name="STEP 1" totalsRowLabel="200"/>
@@ -518,7 +535,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -809,11 +826,11 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D11" sqref="D11:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
@@ -846,7 +863,7 @@
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -887,7 +904,7 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -917,7 +934,7 @@
         <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F7">
         <v>10</v>
@@ -1055,7 +1072,7 @@
         <v>36</v>
       </c>
       <c r="E16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1111,7 +1128,7 @@
         <v>36</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1193,11 +1210,11 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22:D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
@@ -1276,7 +1293,7 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1297,7 +1314,7 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="E7" t="s">
         <v>23</v>
@@ -1317,7 +1334,7 @@
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E8">
         <v>2000</v>
@@ -1337,7 +1354,7 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="E9">
         <v>1.5</v>
@@ -1357,7 +1374,7 @@
         <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="E10" t="s">
         <v>33</v>
@@ -1371,7 +1388,7 @@
         <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="E11">
         <v>10</v>
@@ -1385,7 +1402,7 @@
         <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -1399,7 +1416,7 @@
         <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="E13" t="s">
         <v>32</v>
@@ -1413,7 +1430,7 @@
         <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E14">
         <v>-5</v>
@@ -1427,7 +1444,7 @@
         <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="E15">
         <v>-20.8</v>
@@ -1460,7 +1477,7 @@
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="E19">
         <v>10</v>
@@ -1477,7 +1494,7 @@
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1493,9 +1510,6 @@
       <c r="B21" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D21" t="s">
-        <v>42</v>
-      </c>
       <c r="E21" t="s">
         <v>38</v>
       </c>
@@ -1508,7 +1522,7 @@
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E22">
         <v>2.8</v>
@@ -1525,7 +1539,7 @@
         <v>25</v>
       </c>
       <c r="D23" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -1539,7 +1553,7 @@
         <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F24">
         <v>-25</v>
@@ -1553,7 +1567,7 @@
         <v>27</v>
       </c>
       <c r="D25" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="F25">
         <v>-1.7</v>

</xml_diff>